<commit_message>
CARLA-3 correction of DPE.
</commit_message>
<xml_diff>
--- a/analyst/Ines/rmonize/data_proc_elem/DPE_CARLA_INES.xlsx
+++ b/analyst/Ines/rmonize/data_proc_elem/DPE_CARLA_INES.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perrar\Documents\Perrar\NFDI4Health\TA5_1\use-cases-harmonisation\analyst\Ines\rmonize\data_proc_elem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\use-cases-harmonisation\analyst\Ines\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E12BA5-CE03-4401-9AC7-F1A1BA18B579}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -385,7 +386,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -405,13 +406,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -445,7 +439,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -470,28 +469,24 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -500,15 +495,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -524,7 +523,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -599,6 +598,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -634,6 +650,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -809,21 +842,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="34.90625" customWidth="1"/>
-    <col min="5" max="7" width="8.7265625" customWidth="1"/>
-    <col min="9" max="9" width="17.36328125" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -858,7 +897,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>16</v>
       </c>
@@ -871,7 +910,7 @@
       <c r="E2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>93</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -888,7 +927,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -901,7 +940,7 @@
       <c r="E3" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>94</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -918,7 +957,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>20</v>
       </c>
@@ -931,7 +970,7 @@
       <c r="E4" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>95</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -948,7 +987,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>22</v>
       </c>
@@ -961,7 +1000,7 @@
       <c r="E5" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>96</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -978,7 +1017,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -1009,7 +1048,7 @@
       </c>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>24</v>
       </c>
@@ -1040,7 +1079,7 @@
       </c>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>26</v>
       </c>
@@ -1071,7 +1110,7 @@
       </c>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>28</v>
       </c>
@@ -1102,7 +1141,7 @@
       </c>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>30</v>
       </c>
@@ -1133,7 +1172,7 @@
       </c>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>32</v>
       </c>
@@ -1164,7 +1203,7 @@
       </c>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>34</v>
       </c>
@@ -1195,7 +1234,7 @@
       </c>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>36</v>
       </c>
@@ -1226,7 +1265,7 @@
       </c>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>38</v>
       </c>
@@ -1255,7 +1294,7 @@
       </c>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>40</v>
       </c>
@@ -1284,7 +1323,7 @@
       </c>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>42</v>
       </c>
@@ -1313,7 +1352,7 @@
       </c>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>44</v>
       </c>
@@ -1342,7 +1381,7 @@
       </c>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="2:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>46</v>
       </c>
@@ -1373,611 +1412,611 @@
       </c>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B19" s="4" t="s">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F19" s="11" t="s">
+      <c r="D19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H19" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="J19" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="K19" s="4" t="s">
+      <c r="J19" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K19" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B20" s="4" t="s">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F20" s="11" t="s">
+      <c r="D20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="G20" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B21" s="4" t="s">
+      <c r="G20" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F21" s="11" t="s">
+      <c r="D21" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="G21" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B22" s="4" t="s">
+      <c r="G21" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F22" s="11" t="s">
+      <c r="D22" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="G22" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B23" s="4" t="s">
+      <c r="G22" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F23" s="11" t="s">
+      <c r="D23" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F23" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="G23" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B24" s="4" t="s">
+      <c r="G23" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F24" s="11" t="s">
+      <c r="D24" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="G24" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B25" s="4" t="s">
+      <c r="G24" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K24" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F25" s="11" t="s">
+      <c r="D25" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="G25" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B26" s="4" t="s">
+      <c r="G25" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K25" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F26" s="11" t="s">
+      <c r="D26" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F26" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="G26" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="K26" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B27" s="4" t="s">
+      <c r="G26" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F27" s="11" t="s">
+      <c r="D27" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="G27" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="B28" s="4" t="s">
+      <c r="G27" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B28" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F28" s="11" t="s">
+      <c r="D28" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F28" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="G28" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="H28" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="I28" s="7"/>
-      <c r="J28" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B29" s="4" t="s">
+      <c r="I28" s="11"/>
+      <c r="J28" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K28" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F29" s="11"/>
-      <c r="G29" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="K29" s="4" t="s">
+      <c r="D29" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F29" s="10"/>
+      <c r="G29" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="K29" s="9" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B30" s="4" t="s">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F30" s="11"/>
-      <c r="G30" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="K30" s="4" t="s">
+      <c r="D30" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F30" s="10"/>
+      <c r="G30" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="K30" s="9" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B31" s="4" t="s">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F31" s="11" t="s">
+      <c r="D31" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F31" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="G31" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="K31" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B32" s="4" t="s">
+      <c r="G31" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K31" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" s="4" t="s">
+      <c r="D32" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="9" t="s">
         <v>92</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="G32" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="K32" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B33" s="4" t="s">
+      <c r="G32" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K32" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E33" s="4" t="s">
+      <c r="D33" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="9" t="s">
         <v>92</v>
       </c>
       <c r="F33" s="12"/>
-      <c r="G33" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="K33" s="4" t="s">
+      <c r="G33" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="K33" s="9" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B34" s="4" t="s">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B34" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" s="4" t="s">
+      <c r="D34" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="9" t="s">
         <v>92</v>
       </c>
       <c r="F34" s="12"/>
-      <c r="G34" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="K34" s="4" t="s">
+      <c r="G34" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="K34" s="9" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B35" s="4" t="s">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B35" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E35" s="4" t="s">
+      <c r="D35" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="9" t="s">
         <v>92</v>
       </c>
       <c r="F35" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="G35" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="K35" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B36" s="4" t="s">
+      <c r="G35" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K35" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D36" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F36" s="11" t="s">
+      <c r="D36" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F36" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="G36" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="H36" s="4" t="s">
+      <c r="H36" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="K36" s="4" t="s">
+      <c r="I36" s="9"/>
+      <c r="J36" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K36" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="F37" s="6"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="9"/>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="F38" s="6"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="9"/>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="F39" s="6"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="9"/>
-      <c r="K39" s="9"/>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="F40" s="6"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="9"/>
-      <c r="K40" s="9"/>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="F41" s="6"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="9"/>
-      <c r="K41" s="9"/>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="F42" s="6"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="9"/>
-      <c r="K42" s="9"/>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="F43" s="6"/>
-      <c r="I43" s="8"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="9"/>
-    </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="F44" s="6"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="9"/>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="F45" s="6"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="9"/>
-      <c r="K45" s="9"/>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="F46" s="6"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="9"/>
-    </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="F47" s="6"/>
-      <c r="I47" s="10"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="9"/>
-    </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="F48" s="6"/>
-      <c r="I48" s="10"/>
-      <c r="J48" s="9"/>
-      <c r="K48" s="9"/>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F37" s="5"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F38" s="5"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F39" s="5"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F40" s="5"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F41" s="5"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F42" s="5"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F43" s="5"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F44" s="5"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F45" s="5"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F46" s="5"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F47" s="5"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F48" s="5"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>